<commit_message>
update description document - march 16 covid data
</commit_message>
<xml_diff>
--- a/covid counties/data.xlsx
+++ b/covid counties/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FreeLance\covid19countiesprediction\covid counties\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C99BB33-1EAD-42DC-9DA1-DE46EB0B1B60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE566BBA-8C65-4ED7-9F05-DD6F712B915C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -549,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2:S59"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -583,6 +583,9 @@
       <c r="G1" s="2">
         <v>43915</v>
       </c>
+      <c r="H1" s="2">
+        <v>43916</v>
+      </c>
       <c r="L1" t="s">
         <v>61</v>
       </c>
@@ -618,6 +621,13 @@
       <c r="G2">
         <v>152</v>
       </c>
+      <c r="H2">
+        <v>171</v>
+      </c>
+      <c r="J2">
+        <f>H2-G2</f>
+        <v>19</v>
+      </c>
       <c r="L2">
         <f>G2/B2</f>
         <v>4.9966469868903765E-4</v>
@@ -665,28 +675,35 @@
       <c r="G3">
         <v>2</v>
       </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J59" si="1">H3-G3</f>
+        <v>0</v>
+      </c>
       <c r="L3">
-        <f t="shared" ref="L3:L59" si="1">G3/B3</f>
+        <f t="shared" ref="L3:L59" si="2">G3/B3</f>
         <v>4.0861357414293305E-5</v>
       </c>
       <c r="M3">
-        <f t="shared" ref="M3:M59" si="2">G3/C3</f>
+        <f t="shared" ref="M3:M59" si="3">G3/C3</f>
         <v>1.9342359767891683E-3</v>
       </c>
       <c r="O3">
-        <f t="shared" ref="O3:O59" si="3">(E3-D3)/D3*100</f>
+        <f t="shared" ref="O3:O59" si="4">(E3-D3)/D3*100</f>
         <v>0</v>
       </c>
       <c r="P3">
-        <f t="shared" ref="P3:P59" si="4">(F3-E3)/E3*100</f>
+        <f t="shared" ref="P3:P59" si="5">(F3-E3)/E3*100</f>
         <v>0</v>
       </c>
       <c r="Q3">
-        <f t="shared" ref="Q3:Q59" si="5">(G3-F3)/F3*100</f>
+        <f t="shared" ref="Q3:Q59" si="6">(G3-F3)/F3*100</f>
         <v>0</v>
       </c>
       <c r="S3">
-        <f t="shared" ref="S3:S59" si="6">ROUND(AVERAGE(O3:Q3),0)</f>
+        <f t="shared" ref="S3:S59" si="7">ROUND(AVERAGE(O3:Q3),0)</f>
         <v>0</v>
       </c>
     </row>
@@ -712,28 +729,35 @@
       <c r="G4">
         <v>11</v>
       </c>
+      <c r="H4">
+        <v>16</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
       <c r="L4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.4835493519441675E-5</v>
       </c>
       <c r="M4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.5384615384615385E-2</v>
       </c>
       <c r="O4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>250</v>
       </c>
       <c r="P4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>57.142857142857139</v>
       </c>
       <c r="S4">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>102</v>
       </c>
     </row>
@@ -759,12 +783,19 @@
       <c r="G5">
         <v>0</v>
       </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="L5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O5">
@@ -777,7 +808,7 @@
         <v>0</v>
       </c>
       <c r="S5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -803,27 +834,34 @@
       <c r="G6">
         <v>2</v>
       </c>
+      <c r="H6">
+        <v>2</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="L6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.4991877639767076E-5</v>
       </c>
       <c r="M6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.3148148148148147E-3</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="S6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -849,12 +887,19 @@
       <c r="G7">
         <v>1</v>
       </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="L7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.4126236981579634E-6</v>
       </c>
       <c r="M7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.6666666666666664E-4</v>
       </c>
       <c r="O7">
@@ -867,7 +912,7 @@
         <v>0</v>
       </c>
       <c r="S7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -893,12 +938,19 @@
       <c r="G8">
         <v>1</v>
       </c>
+      <c r="H8">
+        <v>7</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
       <c r="L8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.1257458065968705E-5</v>
       </c>
       <c r="M8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.4342153306881526E-3</v>
       </c>
       <c r="O8">
@@ -911,7 +963,7 @@
         <v>0</v>
       </c>
       <c r="S8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -937,28 +989,35 @@
       <c r="G9">
         <v>3</v>
       </c>
+      <c r="H9">
+        <v>3</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="L9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.9433009093250389E-5</v>
       </c>
       <c r="M9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.3375980419424818E-3</v>
       </c>
       <c r="O9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>50</v>
       </c>
       <c r="P9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="S9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>17</v>
       </c>
     </row>
@@ -984,28 +1043,35 @@
       <c r="G10">
         <v>10</v>
       </c>
+      <c r="H10">
+        <v>11</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
       <c r="L10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.2176115332164427E-4</v>
       </c>
       <c r="M10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8.9445438282647581E-3</v>
       </c>
       <c r="O10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>50</v>
       </c>
       <c r="P10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>66.666666666666657</v>
       </c>
       <c r="S10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>39</v>
       </c>
     </row>
@@ -1031,28 +1097,35 @@
       <c r="G11">
         <v>12</v>
       </c>
+      <c r="H11">
+        <v>13</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
       <c r="L11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.9018638265500191E-4</v>
       </c>
       <c r="M11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.8518518518518517E-2</v>
       </c>
       <c r="O11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>400</v>
       </c>
       <c r="P11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="S11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>140</v>
       </c>
     </row>
@@ -1078,28 +1151,35 @@
       <c r="G12">
         <v>2</v>
       </c>
+      <c r="H12">
+        <v>2</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="L12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.0538349278417384E-5</v>
       </c>
       <c r="M12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.9840637450199202E-3</v>
       </c>
       <c r="O12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="P12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="S12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>33</v>
       </c>
     </row>
@@ -1125,28 +1205,35 @@
       <c r="G13">
         <v>5</v>
       </c>
+      <c r="H13">
+        <v>7</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
       <c r="L13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.0421008753647353E-4</v>
       </c>
       <c r="M13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.4059945504087193E-3</v>
       </c>
       <c r="O13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>200</v>
       </c>
       <c r="P13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>66.666666666666657</v>
       </c>
       <c r="S13">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>89</v>
       </c>
     </row>
@@ -1172,28 +1259,35 @@
       <c r="G14">
         <v>153</v>
       </c>
+      <c r="H14">
+        <v>190</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
       <c r="L14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.1430645942021191E-4</v>
       </c>
       <c r="M14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.18545454545454546</v>
       </c>
       <c r="O14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>104.08163265306123</v>
       </c>
       <c r="P14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>24</v>
       </c>
       <c r="Q14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>23.387096774193548</v>
       </c>
       <c r="S14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>50</v>
       </c>
     </row>
@@ -1219,28 +1313,35 @@
       <c r="G15">
         <v>122</v>
       </c>
+      <c r="H15">
+        <v>134</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
       <c r="L15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.3274721448467967E-4</v>
       </c>
       <c r="M15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9.9429502852485738E-2</v>
       </c>
       <c r="O15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>128.94736842105263</v>
       </c>
       <c r="P15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>22.988505747126435</v>
       </c>
       <c r="Q15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>14.018691588785046</v>
       </c>
       <c r="S15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>55</v>
       </c>
     </row>
@@ -1266,28 +1367,35 @@
       <c r="G16">
         <v>4</v>
       </c>
+      <c r="H16">
+        <v>4</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="L16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.016002032004064E-4</v>
       </c>
       <c r="M16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.0876826722338203E-3</v>
       </c>
       <c r="O16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>50</v>
       </c>
       <c r="P16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>33.333333333333329</v>
       </c>
       <c r="S16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>28</v>
       </c>
     </row>
@@ -1313,12 +1421,19 @@
       <c r="G17">
         <v>1</v>
       </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="L17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.9380220546909824E-5</v>
       </c>
       <c r="M17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.8927519151443723E-4</v>
       </c>
       <c r="O17">
@@ -1331,7 +1446,7 @@
         <v>0</v>
       </c>
       <c r="S17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -1357,28 +1472,35 @@
       <c r="G18">
         <v>1</v>
       </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="L18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.8007959518107003E-5</v>
       </c>
       <c r="M18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.876172607879925E-3</v>
       </c>
       <c r="O18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="P18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="S18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -1404,28 +1526,35 @@
       <c r="G19">
         <v>2</v>
       </c>
+      <c r="H19">
+        <v>4</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
       <c r="L19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.3289502155495265E-5</v>
       </c>
       <c r="M19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4.0404040404040404E-3</v>
       </c>
       <c r="O19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="P19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>100</v>
       </c>
       <c r="S19">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>33</v>
       </c>
     </row>
@@ -1451,28 +1580,35 @@
       <c r="G20">
         <v>4</v>
       </c>
+      <c r="H20">
+        <v>5</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
       <c r="L20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.1266126246927128E-5</v>
       </c>
       <c r="M20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.0790273556231003E-3</v>
       </c>
       <c r="O20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="P20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="S20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>33</v>
       </c>
     </row>
@@ -1498,28 +1634,35 @@
       <c r="G21">
         <v>2</v>
       </c>
+      <c r="H21">
+        <v>2</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="L21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.1356492969396195E-4</v>
       </c>
       <c r="M21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.1061946902654867E-3</v>
       </c>
       <c r="O21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="P21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="S21">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -1545,28 +1688,35 @@
       <c r="G22">
         <v>5</v>
       </c>
+      <c r="H22">
+        <v>7</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
       <c r="L22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.749655140346254E-5</v>
       </c>
       <c r="M22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.4293552812071329E-3</v>
       </c>
       <c r="O22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>33.333333333333329</v>
       </c>
       <c r="P22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>25</v>
       </c>
       <c r="S22">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>19</v>
       </c>
     </row>
@@ -1592,28 +1742,35 @@
       <c r="G23">
         <v>2</v>
       </c>
+      <c r="H23">
+        <v>3</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
       <c r="L23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.7207409510535236E-5</v>
       </c>
       <c r="M23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.0770059235325794E-3</v>
       </c>
       <c r="O23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="P23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="S23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>33</v>
       </c>
     </row>
@@ -1639,12 +1796,19 @@
       <c r="G24">
         <v>0</v>
       </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="L24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O24">
@@ -1657,7 +1821,7 @@
         <v>0</v>
       </c>
       <c r="S24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -1683,28 +1847,35 @@
       <c r="G25">
         <v>3</v>
       </c>
+      <c r="H25">
+        <v>3</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="L25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.5876469958558254E-5</v>
       </c>
       <c r="M25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4.6874999999999998E-3</v>
       </c>
       <c r="O25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>50</v>
       </c>
       <c r="P25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="S25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>17</v>
       </c>
     </row>
@@ -1730,27 +1901,34 @@
       <c r="G26">
         <v>7</v>
       </c>
+      <c r="H26">
+        <v>9</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
       <c r="L26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.5313308461098556E-5</v>
       </c>
       <c r="M26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.0574018126888218E-2</v>
       </c>
       <c r="O26">
         <v>0</v>
       </c>
       <c r="P26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>75</v>
       </c>
       <c r="S26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>25</v>
       </c>
     </row>
@@ -1776,28 +1954,35 @@
       <c r="G27">
         <v>118</v>
       </c>
+      <c r="H27">
+        <v>139</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
       <c r="L27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.585288522511097E-4</v>
       </c>
       <c r="M27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8.6383601756954614E-2</v>
       </c>
       <c r="O27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>80.952380952380949</v>
       </c>
       <c r="P27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>26.315789473684209</v>
       </c>
       <c r="Q27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>22.916666666666664</v>
       </c>
       <c r="S27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43</v>
       </c>
     </row>
@@ -1823,28 +2008,35 @@
       <c r="G28">
         <v>4</v>
       </c>
+      <c r="H28">
+        <v>5</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
       <c r="L28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.9651128059101138E-5</v>
       </c>
       <c r="M28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9.7560975609756097E-3</v>
       </c>
       <c r="O28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="P28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>33.333333333333329</v>
       </c>
       <c r="S28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>11</v>
       </c>
     </row>
@@ -1870,29 +2062,35 @@
       <c r="G29" s="1">
         <v>3285</v>
       </c>
-      <c r="J29" s="1"/>
+      <c r="H29" s="1">
+        <v>3914</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="1"/>
+        <v>629</v>
+      </c>
       <c r="L29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.4523490293624937E-3</v>
       </c>
       <c r="M29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.2516556291390728</v>
       </c>
       <c r="O29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>97.893030794165313</v>
       </c>
       <c r="P29">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>17.485667485667484</v>
       </c>
       <c r="Q29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>14.499825723248518</v>
       </c>
       <c r="S29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>43</v>
       </c>
     </row>
@@ -1918,29 +2116,35 @@
       <c r="G30">
         <v>12</v>
       </c>
-      <c r="J30" s="1"/>
+      <c r="H30">
+        <v>14</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
       <c r="L30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.5435189334269569E-5</v>
       </c>
       <c r="M30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.0526315789473684E-2</v>
       </c>
       <c r="O30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>150</v>
       </c>
       <c r="P30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q30">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="S30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>57</v>
       </c>
     </row>
@@ -1966,28 +2170,35 @@
       <c r="G31">
         <v>9</v>
       </c>
+      <c r="H31">
+        <v>13</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
       <c r="L31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.8317764967344751E-5</v>
       </c>
       <c r="M31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.4196207749381701E-3</v>
       </c>
       <c r="O31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>75</v>
       </c>
       <c r="P31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>28.571428571428569</v>
       </c>
       <c r="S31">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>35</v>
       </c>
     </row>
@@ -2013,28 +2224,35 @@
       <c r="G32">
         <v>65</v>
       </c>
+      <c r="H32">
+        <v>83</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
       <c r="L32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.3917854680467467E-4</v>
       </c>
       <c r="M32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8.0645161290322578E-2</v>
       </c>
       <c r="O32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>205.88235294117646</v>
       </c>
       <c r="P32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>25</v>
       </c>
       <c r="S32">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>77</v>
       </c>
     </row>
@@ -2060,28 +2278,35 @@
       <c r="G33">
         <v>9</v>
       </c>
+      <c r="H33">
+        <v>11</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
       <c r="L33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.3386608110737416E-5</v>
       </c>
       <c r="M33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.3595166163141994E-2</v>
       </c>
       <c r="O33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>50</v>
       </c>
       <c r="P33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>50</v>
       </c>
       <c r="S33">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>33</v>
       </c>
     </row>
@@ -2107,28 +2332,35 @@
       <c r="G34">
         <v>638</v>
       </c>
+      <c r="H34">
+        <v>751</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="1"/>
+        <v>113</v>
+      </c>
       <c r="L34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.7113137149187393E-3</v>
       </c>
       <c r="M34">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.76042908224076278</v>
       </c>
       <c r="O34">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>138.65030674846625</v>
       </c>
       <c r="P34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>28.020565552699228</v>
       </c>
       <c r="Q34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>28.112449799196789</v>
       </c>
       <c r="S34">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>65</v>
       </c>
     </row>
@@ -2154,12 +2386,19 @@
       <c r="G35">
         <v>2</v>
       </c>
+      <c r="H35">
+        <v>2</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="L35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.6638528088053541E-5</v>
       </c>
       <c r="M35">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.4479804161566705E-3</v>
       </c>
       <c r="O35">
@@ -2172,7 +2411,7 @@
         <v>0</v>
       </c>
       <c r="S35">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -2198,27 +2437,34 @@
       <c r="G36">
         <v>2</v>
       </c>
+      <c r="H36">
+        <v>4</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
       <c r="L36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.6378809096790571E-5</v>
       </c>
       <c r="M36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.5243902439024391E-3</v>
       </c>
       <c r="O36">
         <v>0</v>
       </c>
       <c r="P36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>100</v>
       </c>
       <c r="S36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>33</v>
       </c>
     </row>
@@ -2244,27 +2490,34 @@
       <c r="G37">
         <v>2</v>
       </c>
+      <c r="H37">
+        <v>3</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
       <c r="L37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.2123869641336994E-5</v>
       </c>
       <c r="M37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.9940179461615153E-3</v>
       </c>
       <c r="O37">
         <v>0</v>
       </c>
       <c r="P37">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>100</v>
       </c>
       <c r="S37">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>33</v>
       </c>
     </row>
@@ -2290,28 +2543,35 @@
       <c r="G38">
         <v>84</v>
       </c>
+      <c r="H38">
+        <v>94</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
       <c r="L38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.4244308494634435E-4</v>
       </c>
       <c r="M38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.34146341463414637</v>
       </c>
       <c r="O38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>104.54545454545455</v>
       </c>
       <c r="P38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>86.666666666666671</v>
       </c>
       <c r="S38">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>64</v>
       </c>
     </row>
@@ -2337,28 +2597,35 @@
       <c r="G39">
         <v>31</v>
       </c>
+      <c r="H39">
+        <v>32</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
       <c r="L39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.9444392174573007E-4</v>
       </c>
       <c r="M39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4.6616541353383459E-2</v>
       </c>
       <c r="O39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>45</v>
       </c>
       <c r="P39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6.8965517241379306</v>
       </c>
       <c r="S39">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>17</v>
       </c>
     </row>
@@ -2384,28 +2651,35 @@
       <c r="G40">
         <v>968</v>
       </c>
+      <c r="H40">
+        <v>1197</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="1"/>
+        <v>229</v>
+      </c>
       <c r="L40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.105679736402224E-3</v>
       </c>
       <c r="M40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4.8643216080402008</v>
       </c>
       <c r="O40">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>125.95419847328245</v>
       </c>
       <c r="P40">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>13.344594594594595</v>
       </c>
       <c r="Q40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44.26229508196721</v>
       </c>
       <c r="S40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>61</v>
       </c>
     </row>
@@ -2431,27 +2705,34 @@
       <c r="G41">
         <v>1</v>
       </c>
+      <c r="H41">
+        <v>2</v>
+      </c>
+      <c r="J41">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
       <c r="L41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.9330379475452008E-6</v>
       </c>
       <c r="M41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.5448422545196739E-4</v>
       </c>
       <c r="O41">
         <v>0</v>
       </c>
       <c r="P41">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="S41">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -2477,28 +2758,35 @@
       <c r="G42">
         <v>64</v>
       </c>
+      <c r="H42">
+        <v>73</v>
+      </c>
+      <c r="J42">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
       <c r="L42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.9142969031041815E-4</v>
       </c>
       <c r="M42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.582938388625593E-2</v>
       </c>
       <c r="O42">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>51.428571428571423</v>
       </c>
       <c r="P42">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>20.754716981132077</v>
       </c>
       <c r="S42">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>24</v>
       </c>
     </row>
@@ -2524,28 +2812,35 @@
       <c r="G43">
         <v>55</v>
       </c>
+      <c r="H43">
+        <v>62</v>
+      </c>
+      <c r="J43">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
       <c r="L43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.5546478636566339E-4</v>
       </c>
       <c r="M43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.26190476190476192</v>
       </c>
       <c r="O43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>37.5</v>
       </c>
       <c r="P43">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>25</v>
       </c>
       <c r="S43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>21</v>
       </c>
     </row>
@@ -2571,28 +2866,35 @@
       <c r="G44">
         <v>2</v>
       </c>
+      <c r="H44">
+        <v>2</v>
+      </c>
+      <c r="J44">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="L44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.1070567040214963E-5</v>
       </c>
       <c r="M44">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.1948881789137379E-3</v>
       </c>
       <c r="O44">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="P44">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q44">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>100</v>
       </c>
       <c r="S44">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>33</v>
       </c>
     </row>
@@ -2618,12 +2920,19 @@
       <c r="G45">
         <v>0</v>
       </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="J45">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="L45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M45">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O45">
@@ -2636,7 +2945,7 @@
         <v>0</v>
       </c>
       <c r="S45">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -2662,12 +2971,19 @@
       <c r="G46">
         <v>0</v>
       </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="J46">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="L46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M46">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O46">
@@ -2680,7 +2996,7 @@
         <v>0</v>
       </c>
       <c r="S46">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -2706,28 +3022,35 @@
       <c r="G47">
         <v>8</v>
       </c>
+      <c r="H47">
+        <v>11</v>
+      </c>
+      <c r="J47">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
       <c r="L47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.0816244065057071E-5</v>
       </c>
       <c r="M47">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6980056980056983E-3</v>
       </c>
       <c r="O47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="P47">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q47">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>100</v>
       </c>
       <c r="S47">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>67</v>
       </c>
     </row>
@@ -2753,29 +3076,35 @@
       <c r="G48" s="1">
         <v>2260</v>
       </c>
-      <c r="J48" s="1"/>
+      <c r="H48" s="1">
+        <v>2735</v>
+      </c>
+      <c r="J48">
+        <f t="shared" si="1"/>
+        <v>475</v>
+      </c>
       <c r="L48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.513375966786085E-3</v>
       </c>
       <c r="M48">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.95238095238095233</v>
       </c>
       <c r="O48">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>120.24169184290029</v>
       </c>
       <c r="P48">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>28.943758573388202</v>
       </c>
       <c r="Q48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>20.212765957446805</v>
       </c>
       <c r="S48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>56</v>
       </c>
     </row>
@@ -2801,28 +3130,35 @@
       <c r="G49">
         <v>39</v>
       </c>
+      <c r="H49">
+        <v>53</v>
+      </c>
+      <c r="J49">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
       <c r="L49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.0292080931564089E-4</v>
       </c>
       <c r="M49">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.9117352056168508E-2</v>
       </c>
       <c r="O49">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>91.666666666666657</v>
       </c>
       <c r="P49">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q49">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>69.565217391304344</v>
       </c>
       <c r="S49">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>54</v>
       </c>
     </row>
@@ -2848,28 +3184,35 @@
       <c r="G50">
         <v>1</v>
       </c>
+      <c r="H50">
+        <v>2</v>
+      </c>
+      <c r="J50">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
       <c r="L50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.9559902200488996E-5</v>
       </c>
       <c r="M50">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.9120458891013384E-3</v>
       </c>
       <c r="O50">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="P50">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q50">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="S50">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -2895,28 +3238,35 @@
       <c r="G51">
         <v>16</v>
       </c>
+      <c r="H51">
+        <v>22</v>
+      </c>
+      <c r="J51">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
       <c r="L51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.5753613485093142E-4</v>
       </c>
       <c r="M51">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.3613445378151259E-2</v>
       </c>
       <c r="O51">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>36.363636363636367</v>
       </c>
       <c r="P51">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q51">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6.666666666666667</v>
       </c>
       <c r="S51">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>14</v>
       </c>
     </row>
@@ -2942,28 +3292,35 @@
       <c r="G52">
         <v>65</v>
       </c>
+      <c r="H52">
+        <v>78</v>
+      </c>
+      <c r="J52">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
       <c r="L52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.5617804518529476E-4</v>
       </c>
       <c r="M52">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.5986218776916452E-2</v>
       </c>
       <c r="O52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>94.444444444444443</v>
       </c>
       <c r="P52">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q52">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>85.714285714285708</v>
       </c>
       <c r="S52">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>60</v>
       </c>
     </row>
@@ -2989,28 +3346,35 @@
       <c r="G53">
         <v>2</v>
       </c>
+      <c r="H53">
+        <v>2</v>
+      </c>
+      <c r="J53">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="L53">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.0438157273958636E-5</v>
       </c>
       <c r="M53">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.2988505747126436E-3</v>
       </c>
       <c r="O53">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="P53">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q53">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="S53">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>33</v>
       </c>
     </row>
@@ -3036,28 +3400,35 @@
       <c r="G54">
         <v>4</v>
       </c>
+      <c r="H54">
+        <v>4</v>
+      </c>
+      <c r="J54">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="L54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.3275120222728426E-5</v>
       </c>
       <c r="M54">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4.7281323877068557E-3</v>
       </c>
       <c r="O54">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>200</v>
       </c>
       <c r="P54">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q54">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>33.333333333333329</v>
       </c>
       <c r="S54">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>78</v>
       </c>
     </row>
@@ -3083,28 +3454,35 @@
       <c r="G55">
         <v>7</v>
       </c>
+      <c r="H55">
+        <v>8</v>
+      </c>
+      <c r="J55">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
       <c r="L55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.4649148999701408E-5</v>
       </c>
       <c r="M55">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.0578034682080926E-3</v>
       </c>
       <c r="O55">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="P55">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q55">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>16.666666666666664</v>
       </c>
       <c r="S55">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>39</v>
       </c>
     </row>
@@ -3130,28 +3508,35 @@
       <c r="G56" s="1">
         <v>4691</v>
       </c>
+      <c r="H56" s="1">
+        <v>5944</v>
+      </c>
+      <c r="J56">
+        <f t="shared" si="1"/>
+        <v>1253</v>
+      </c>
       <c r="L56">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.9425094799038678E-3</v>
       </c>
       <c r="M56">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9.3819999999999997</v>
       </c>
       <c r="O56">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>108.65176640230713</v>
       </c>
       <c r="P56">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>34.450587422252937</v>
       </c>
       <c r="Q56">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>20.560267283474683</v>
       </c>
       <c r="S56">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>55</v>
       </c>
     </row>
@@ -3177,28 +3562,35 @@
       <c r="G57">
         <v>4</v>
       </c>
+      <c r="H57">
+        <v>7</v>
+      </c>
+      <c r="J57">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
       <c r="L57">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.4887913651998582E-5</v>
       </c>
       <c r="M57">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.7114093959731542E-3</v>
       </c>
       <c r="O57">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="P57">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="Q57">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="S57">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>33</v>
       </c>
     </row>
@@ -3224,12 +3616,19 @@
       <c r="G58">
         <v>0</v>
       </c>
+      <c r="H58">
+        <v>0</v>
+      </c>
+      <c r="J58">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
       <c r="L58">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M58">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O58">
@@ -3242,7 +3641,7 @@
         <v>0</v>
       </c>
       <c r="S58">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
@@ -3268,30 +3667,40 @@
       <c r="G59">
         <v>17856</v>
       </c>
+      <c r="H59">
+        <v>21393</v>
+      </c>
+      <c r="J59">
+        <f t="shared" si="1"/>
+        <v>3537</v>
+      </c>
       <c r="L59">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2.1841846487390482E-3</v>
       </c>
       <c r="M59">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>38.08223852584883</v>
       </c>
       <c r="O59">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>98.116245371115767</v>
       </c>
       <c r="P59">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>21.121495327102803</v>
       </c>
       <c r="Q59">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>19.806763285024154</v>
       </c>
       <c r="S59">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>46</v>
       </c>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="I61" s="1"/>
     </row>
     <row r="70" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E70" s="1"/>

</xml_diff>